<commit_message>
Adding Log4j to POM + Log4j configuration file
</commit_message>
<xml_diff>
--- a/SeleniumDataDrivenFramework/src/test/resources/testData/testdata.xlsx
+++ b/SeleniumDataDrivenFramework/src/test/resources/testData/testdata.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\SeleniumAutomation\SeleniumDataDrivenFramework\src\test\resources\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\SeleniumAutomation\AutomationTestingPlayground\SeleniumDataDrivenFramework\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367B04D2-4EBB-4519-B1A9-588F2D92D002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD12891-C835-40BB-992D-DF92A9D9535E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24765" yWindow="4800" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="900" windowWidth="8745" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="loginTest" sheetId="1" r:id="rId1"/>
+    <sheet name="loginAsBankManager" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>username</t>
   </si>
@@ -357,7 +357,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -385,14 +385,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding basic ReportNG funcionality to test suite
</commit_message>
<xml_diff>
--- a/SeleniumDataDrivenFramework/src/test/resources/testData/testdata.xlsx
+++ b/SeleniumDataDrivenFramework/src/test/resources/testData/testdata.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\SeleniumAutomation\AutomationTestingPlayground\SeleniumDataDrivenFramework\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD12891-C835-40BB-992D-DF92A9D9535E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A95556B-1F5E-4000-90A2-2C418FABDC04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="900" windowWidth="8745" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="loginAsBankManager" sheetId="1" r:id="rId1"/>
+    <sheet name="addCustomer" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,18 +25,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>Add valid username to testdata.xlsx</t>
-  </si>
-  <si>
-    <t>Add valid password to testdata.xlsx</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>postcode</t>
+  </si>
+  <si>
+    <t>Raman</t>
+  </si>
+  <si>
+    <t>Arora</t>
+  </si>
+  <si>
+    <t>A234wd</t>
+  </si>
+  <si>
+    <t>alerttext</t>
+  </si>
+  <si>
+    <t>Customer added successfully with customer id</t>
   </si>
 </sst>
 </file>
@@ -357,32 +369,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="42.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding open account test case
</commit_message>
<xml_diff>
--- a/SeleniumDataDrivenFramework/src/test/resources/testData/testdata.xlsx
+++ b/SeleniumDataDrivenFramework/src/test/resources/testData/testdata.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\SeleniumAutomation\AutomationTestingPlayground\SeleniumDataDrivenFramework\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A95556B-1F5E-4000-90A2-2C418FABDC04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8D6211-ECFB-44CE-A98F-183350C8B545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="900" windowWidth="8745" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="addCustomer" sheetId="1" r:id="rId1"/>
+    <sheet name="OpenAccount" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>firstname</t>
   </si>
@@ -45,10 +46,34 @@
     <t>A234wd</t>
   </si>
   <si>
-    <t>alerttext</t>
-  </si>
-  <si>
-    <t>Customer added successfully with customer id</t>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Rupee</t>
+  </si>
+  <si>
+    <t>Hermoine Granger</t>
+  </si>
+  <si>
+    <t>Roger</t>
+  </si>
+  <si>
+    <t>Gregor</t>
+  </si>
+  <si>
+    <t>Rodrigues</t>
+  </si>
+  <si>
+    <t>Hamon</t>
+  </si>
+  <si>
+    <t>Soraya</t>
+  </si>
+  <si>
+    <t>Khaloy</t>
   </si>
 </sst>
 </file>
@@ -369,19 +394,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="42.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -391,11 +417,8 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -405,11 +428,70 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>652345</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>6646753</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>3425131</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C84580AA-2F99-4EC4-9ED3-7C1731320122}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Setting up run modes for test suites
Now there's a 'test_suite' sheet on the 'testdata.xlsx' and by putting Y or N on the suites the developer is able to run a specific set of tests.
</commit_message>
<xml_diff>
--- a/SeleniumDataDrivenFramework/src/test/resources/testData/testdata.xlsx
+++ b/SeleniumDataDrivenFramework/src/test/resources/testData/testdata.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\SeleniumAutomation\AutomationTestingPlayground\SeleniumDataDrivenFramework\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8D6211-ECFB-44CE-A98F-183350C8B545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204A07EC-3289-41A0-A40B-03F7E0B7F6DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="900" windowWidth="8745" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="addCustomer" sheetId="1" r:id="rId1"/>
-    <sheet name="OpenAccount" sheetId="2" r:id="rId2"/>
+    <sheet name="test_suite" sheetId="3" r:id="rId1"/>
+    <sheet name="addCustomer" sheetId="1" r:id="rId2"/>
+    <sheet name="OpenAccount" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>firstname</t>
   </si>
@@ -74,6 +75,30 @@
   </si>
   <si>
     <t>Khaloy</t>
+  </si>
+  <si>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>Runmode</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>BankManagerLogin</t>
+  </si>
+  <si>
+    <t>AddCustomer</t>
+  </si>
+  <si>
+    <t>CustomerLogin</t>
+  </si>
+  <si>
+    <t>OpenAccount</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -109,11 +134,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,11 +419,66 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF53294B-DE3F-45C1-8444-83838213B6CB}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,7 +548,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C84580AA-2F99-4EC4-9ED3-7C1731320122}">
   <dimension ref="A1:B2"/>
   <sheetViews>

</xml_diff>

<commit_message>
Setup run modes for each test data
Now there's a column 'runmode' on each test data sheet, and the developer can define which test data will be executed by changing the runmode cell value from Y to N or vice versa
</commit_message>
<xml_diff>
--- a/SeleniumDataDrivenFramework/src/test/resources/testData/testdata.xlsx
+++ b/SeleniumDataDrivenFramework/src/test/resources/testData/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\SeleniumAutomation\AutomationTestingPlayground\SeleniumDataDrivenFramework\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204A07EC-3289-41A0-A40B-03F7E0B7F6DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B3BD91-397D-48BD-84AF-A581653FA69A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>firstname</t>
   </si>
@@ -98,7 +98,7 @@
     <t>OpenAccount</t>
   </si>
   <si>
-    <t>N</t>
+    <t>runmode</t>
   </si>
 </sst>
 </file>
@@ -423,7 +423,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,7 +449,7 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -475,10 +475,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,7 +488,7 @@
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -498,8 +498,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -509,8 +512,11 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -520,19 +526,25 @@
       <c r="C3">
         <v>652345</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>6646753</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -541,6 +553,9 @@
       </c>
       <c r="C5">
         <v>3425131</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -550,26 +565,34 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C84580AA-2F99-4EC4-9ED3-7C1731320122}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>